<commit_message>
add token when login
</commit_message>
<xml_diff>
--- a/doc/Excel/MainTable.xlsx
+++ b/doc/Excel/MainTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17940"/>
+    <workbookView windowWidth="26835" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>主表</t>
   </si>
   <si>
+    <t>副表</t>
+  </si>
+  <si>
     <t>数据名称</t>
   </si>
   <si>
@@ -36,6 +39,9 @@
     <t>长度</t>
   </si>
   <si>
+    <t>一级名称</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -45,6 +51,15 @@
     <t>主id</t>
   </si>
   <si>
+    <t>坐标系</t>
+  </si>
+  <si>
+    <t>xAxis</t>
+  </si>
+  <si>
+    <t>X轴坐标</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -54,12 +69,24 @@
     <t>用户名</t>
   </si>
   <si>
+    <t>yAxis</t>
+  </si>
+  <si>
+    <t>Y轴坐标</t>
+  </si>
+  <si>
     <t>password</t>
   </si>
   <si>
     <t>密码</t>
   </si>
   <si>
+    <t>zAxis</t>
+  </si>
+  <si>
+    <t>Z轴坐标</t>
+  </si>
+  <si>
     <t>nickname</t>
   </si>
   <si>
@@ -157,18 +184,6 @@
   </si>
   <si>
     <t>关联用户</t>
-  </si>
-  <si>
-    <t>xAxis</t>
-  </si>
-  <si>
-    <t>X轴坐标</t>
-  </si>
-  <si>
-    <t>yAxis</t>
-  </si>
-  <si>
-    <t>Y轴坐标</t>
   </si>
 </sst>
 </file>
@@ -178,8 +193,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -198,7 +213,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
       <charset val="134"/>
@@ -210,6 +225,89 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -220,19 +318,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -241,114 +356,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,25 +378,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,157 +558,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,6 +569,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -576,21 +621,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -601,32 +631,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,6 +658,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -662,149 +677,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -816,6 +831,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1165,274 +1183,319 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15.175" customWidth="1"/>
     <col min="2" max="2" width="12.3416666666667" customWidth="1"/>
     <col min="3" max="3" width="15.0083333333333" customWidth="1"/>
     <col min="4" max="4" width="27.0083333333333" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="10" width="13.375" customWidth="1"/>
+    <col min="11" max="11" width="11.875" customWidth="1"/>
+    <col min="12" max="13" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28.5" customHeight="1" spans="1:4">
+    <row r="1" ht="28.5" customHeight="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" ht="22.5" customHeight="1" spans="1:5">
+      <c r="E1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" ht="22.5" customHeight="1" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" ht="22.5" customHeight="1" spans="1:4">
+      <c r="M2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="22.5" customHeight="1" spans="1:12">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" ht="22.5" customHeight="1" spans="1:4">
+      <c r="H3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" ht="22.5" customHeight="1" spans="1:12">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" ht="22.5" customHeight="1" spans="1:4">
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" ht="22.5" customHeight="1" spans="1:11">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" ht="22.5" customHeight="1" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" ht="22.5" customHeight="1" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" ht="22.5" customHeight="1" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" ht="22.5" customHeight="1" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" ht="22.5" customHeight="1" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" ht="22.5" customHeight="1" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" ht="22.5" customHeight="1" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" ht="22.5" customHeight="1" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1" spans="1:4">
       <c r="A14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" ht="22.5" customHeight="1" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" ht="22.5" customHeight="1" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" ht="22.5" customHeight="1" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" ht="22.5" customHeight="1" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" ht="22.5" customHeight="1" spans="1:4">
-      <c r="A19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" ht="22.5" customHeight="1" spans="1:4">
-      <c r="A20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="3"/>
-    </row>
+    <row r="19" ht="22.5" customHeight="1"/>
+    <row r="20" ht="22.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="H3:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>